<commit_message>
Reserve and emissions update
</commit_message>
<xml_diff>
--- a/Data/Generators.xlsx
+++ b/Data/Generators.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Dispatchable_2022" sheetId="1" r:id="rId1"/>
-    <sheet name="Nuclear_2022" sheetId="2" r:id="rId2"/>
+    <sheet name="Dispatchable_2023" sheetId="1" r:id="rId1"/>
+    <sheet name="Nuclear_2023" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -215,7 +215,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -231,6 +231,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -240,7 +247,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -248,14 +255,40 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -538,492 +571,492 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="4" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2">
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1">
         <v>1148.4000000000001</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="1">
         <v>44</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="1">
         <v>2375.3989999999999</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3">
+      <c r="C3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1">
         <v>413.6</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="1">
         <v>47</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="1">
         <v>2144.04</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4">
+      <c r="C4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="1">
         <v>2491.1999999999998</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="1">
         <v>37</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="1">
         <v>1961.67</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5">
+      <c r="C5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="1">
         <v>1530.5</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="1">
         <v>35</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="1">
         <v>1967.268</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6">
+      <c r="C6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="1">
         <v>2119</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="1">
         <v>39</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="1">
         <v>2035.088</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7">
+      <c r="C7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="1">
         <v>763.2</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="1">
         <v>45</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="1">
         <v>2348.8240000000001</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8">
+      <c r="C8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="1">
         <v>2558.1999999999998</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="1">
         <v>38</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="1">
         <v>2034.134</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="1">
         <v>423.5</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="1">
         <v>32</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="1">
         <v>2144.04</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="1">
         <v>697.9</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="1">
         <v>19</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="1">
         <v>818.39</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="1">
         <v>697.9</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="1">
         <v>22</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="1">
         <v>840.07600000000002</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="1">
         <v>583.20000000000005</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="1">
         <v>40</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="1">
         <v>1724.951</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="1">
         <v>920</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="1">
         <v>23</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="1">
         <v>964.87300000000005</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="A14" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="1">
         <v>1753.6</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="1">
         <v>46</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="1">
         <v>1971.32</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="A15" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="1">
         <v>799.2</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="1">
         <v>36</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="1">
         <v>1493.624</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="A16" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="1">
         <v>977.5</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="1">
         <v>30</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="1">
         <v>1240.6859999999999</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="A17" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="1">
         <v>2244.8000000000002</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="1">
         <v>24</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="1">
         <v>982.976</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="A18" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="1">
         <v>730</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="1">
         <v>21</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="1">
         <v>835.70100000000002</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="A19" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="1">
         <v>271.2</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="1">
         <v>33</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="1">
         <v>1367.6389999999999</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="A20" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="1">
         <v>979.7</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="1">
         <v>31</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="1">
         <v>1282.9780000000001</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+      <c r="A21" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="1">
         <v>670</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="1">
         <v>25</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="1">
         <v>7200</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="1">
         <v>3</v>
       </c>
     </row>
@@ -1036,170 +1069,170 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D2" s="1">
-        <v>2410.1999999999998</v>
-      </c>
-      <c r="E2">
-        <v>12.2</v>
-      </c>
-      <c r="F2">
+      <c r="D2" s="5">
+        <v>2410</v>
+      </c>
+      <c r="E2" s="1">
+        <v>12</v>
+      </c>
+      <c r="F2" s="1">
         <v>0</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="1">
-        <v>2440.6</v>
-      </c>
-      <c r="E3">
-        <v>12.2</v>
-      </c>
-      <c r="F3">
+      <c r="D3" s="5">
+        <v>2500</v>
+      </c>
+      <c r="E3" s="1">
+        <v>12</v>
+      </c>
+      <c r="F3" s="1">
         <v>0</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D4" s="1">
-        <v>2666.7</v>
-      </c>
-      <c r="E4">
-        <v>12.2</v>
-      </c>
-      <c r="F4">
+      <c r="D4" s="5">
+        <v>2800</v>
+      </c>
+      <c r="E4" s="1">
+        <v>12</v>
+      </c>
+      <c r="F4" s="1">
         <v>0</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D5" s="1">
-        <v>2003.2</v>
-      </c>
-      <c r="E5">
-        <v>12.2</v>
-      </c>
-      <c r="F5">
+      <c r="D5" s="5">
+        <v>2882.2</v>
+      </c>
+      <c r="E5" s="1">
+        <v>12</v>
+      </c>
+      <c r="F5" s="1">
         <v>0</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="1">
         <v>768.6</v>
       </c>
-      <c r="E6">
-        <v>12.2</v>
-      </c>
-      <c r="F6">
+      <c r="E6" s="1">
+        <v>12</v>
+      </c>
+      <c r="F6" s="1">
         <v>0</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="1">
         <v>950.9</v>
       </c>
-      <c r="E7">
-        <v>12.2</v>
-      </c>
-      <c r="F7">
+      <c r="E7" s="1">
+        <v>12</v>
+      </c>
+      <c r="F7" s="1">
         <v>0</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="1">
         <v>3</v>
       </c>
     </row>

</xml_diff>